<commit_message>
Mise ├á jour de l'application
</commit_message>
<xml_diff>
--- a/Metadonnees.xlsx
+++ b/Metadonnees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk69074\Projet python\depot_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A680C7-B084-47D6-A07B-F94F96EC74E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA67B47-A693-410F-BEA4-5EA6C98482E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0AAFE56-323A-4AA3-A453-F318071692D0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12390" uniqueCount="1674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12390" uniqueCount="1676">
   <si>
     <t>Cat_naturaliste</t>
   </si>
@@ -5073,6 +5073,12 @@
   </si>
   <si>
     <t>La zone précisée sur le plan correspondera au périmètre identifié comme territoire de l'espèce par des experts naturalistes. Faire remonter la clause via la fiche désignation ou chantier selon les cas. Espèce très rare. Contacter SEAP.</t>
+  </si>
+  <si>
+    <t>Si nidification de Pic vert localisée, consigne de martelage : réserver l'abre porteur de nid en arbre bio. Ne pas créer de cloisonnement sur la trajectoire de l'arbre en question.</t>
+  </si>
+  <si>
+    <t>Si nidification de Pic épeiche localisée, consigne de martelage : réserver l'abre porteur de nid en arbre bio. Ne pas créer de cloisonnement sur la trajectoire de l'arbre en question.</t>
   </si>
 </sst>
 </file>
@@ -5446,8 +5452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DFB322-0C0C-4C14-830F-4BADDD5E88B6}">
   <dimension ref="A1:AD492"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D496" sqref="D496"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A495" sqref="A1:XFD495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9971,22 +9977,22 @@
         <v>827</v>
       </c>
       <c r="B50">
-        <v>94567</v>
+        <v>95561</v>
       </c>
       <c r="C50" t="s">
         <v>816</v>
       </c>
       <c r="D50" t="s">
-        <v>845</v>
+        <v>883</v>
       </c>
       <c r="E50" t="s">
-        <v>846</v>
+        <v>884</v>
       </c>
       <c r="F50" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="G50" t="s">
-        <v>1116</v>
+        <v>1120</v>
       </c>
       <c r="H50" t="s">
         <v>46</v>
@@ -10004,7 +10010,7 @@
         <v>2</v>
       </c>
       <c r="M50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N50" t="s">
         <v>528</v>
@@ -10013,7 +10019,7 @@
         <v>528</v>
       </c>
       <c r="P50" t="s">
-        <v>528</v>
+        <v>838</v>
       </c>
       <c r="Q50" t="s">
         <v>528</v>
@@ -10022,13 +10028,13 @@
         <v>528</v>
       </c>
       <c r="S50" t="s">
-        <v>528</v>
+        <v>72</v>
       </c>
       <c r="T50" t="s">
-        <v>528</v>
+        <v>48</v>
       </c>
       <c r="U50" t="s">
-        <v>528</v>
+        <v>33</v>
       </c>
       <c r="V50" t="s">
         <v>1118</v>
@@ -10063,31 +10069,31 @@
         <v>827</v>
       </c>
       <c r="B51">
-        <v>95561</v>
+        <v>88472</v>
       </c>
       <c r="C51" t="s">
         <v>816</v>
       </c>
       <c r="D51" t="s">
-        <v>883</v>
+        <v>828</v>
       </c>
       <c r="E51" t="s">
-        <v>884</v>
+        <v>829</v>
       </c>
       <c r="F51" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="G51" t="s">
-        <v>1120</v>
+        <v>830</v>
       </c>
       <c r="H51" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="I51" t="s">
         <v>52</v>
       </c>
       <c r="J51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -10105,10 +10111,10 @@
         <v>528</v>
       </c>
       <c r="P51" t="s">
-        <v>838</v>
+        <v>528</v>
       </c>
       <c r="Q51" t="s">
-        <v>528</v>
+        <v>831</v>
       </c>
       <c r="R51" t="s">
         <v>528</v>
@@ -10123,7 +10129,7 @@
         <v>33</v>
       </c>
       <c r="V51" t="s">
-        <v>1118</v>
+        <v>1664</v>
       </c>
       <c r="W51" t="s">
         <v>74</v>
@@ -10155,22 +10161,22 @@
         <v>827</v>
       </c>
       <c r="B52">
-        <v>88472</v>
+        <v>124699</v>
       </c>
       <c r="C52" t="s">
         <v>816</v>
       </c>
       <c r="D52" t="s">
-        <v>828</v>
+        <v>842</v>
       </c>
       <c r="E52" t="s">
-        <v>829</v>
+        <v>843</v>
       </c>
       <c r="F52" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="G52" t="s">
-        <v>830</v>
+        <v>844</v>
       </c>
       <c r="H52" t="s">
         <v>27</v>
@@ -10191,16 +10197,16 @@
         <v>2</v>
       </c>
       <c r="N52" t="s">
-        <v>528</v>
+        <v>45</v>
       </c>
       <c r="O52" t="s">
         <v>528</v>
       </c>
       <c r="P52" t="s">
-        <v>528</v>
+        <v>838</v>
       </c>
       <c r="Q52" t="s">
-        <v>831</v>
+        <v>528</v>
       </c>
       <c r="R52" t="s">
         <v>528</v>
@@ -10215,7 +10221,7 @@
         <v>33</v>
       </c>
       <c r="V52" t="s">
-        <v>1664</v>
+        <v>1118</v>
       </c>
       <c r="W52" t="s">
         <v>74</v>
@@ -10247,7 +10253,7 @@
         <v>827</v>
       </c>
       <c r="B53">
-        <v>124699</v>
+        <v>82286</v>
       </c>
       <c r="C53" t="s">
         <v>816</v>
@@ -10259,10 +10265,10 @@
         <v>843</v>
       </c>
       <c r="F53" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="G53" t="s">
-        <v>844</v>
+        <v>850</v>
       </c>
       <c r="H53" t="s">
         <v>27</v>
@@ -10283,19 +10289,19 @@
         <v>2</v>
       </c>
       <c r="N53" t="s">
-        <v>45</v>
+        <v>528</v>
       </c>
       <c r="O53" t="s">
         <v>528</v>
       </c>
       <c r="P53" t="s">
-        <v>838</v>
+        <v>528</v>
       </c>
       <c r="Q53" t="s">
         <v>528</v>
       </c>
       <c r="R53" t="s">
-        <v>528</v>
+        <v>819</v>
       </c>
       <c r="S53" t="s">
         <v>72</v>
@@ -10307,7 +10313,7 @@
         <v>33</v>
       </c>
       <c r="V53" t="s">
-        <v>1118</v>
+        <v>1663</v>
       </c>
       <c r="W53" t="s">
         <v>74</v>
@@ -10339,22 +10345,22 @@
         <v>827</v>
       </c>
       <c r="B54">
-        <v>82286</v>
+        <v>115282</v>
       </c>
       <c r="C54" t="s">
         <v>816</v>
       </c>
       <c r="D54" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="E54" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="F54" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="G54" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="H54" t="s">
         <v>27</v>
@@ -10384,10 +10390,10 @@
         <v>528</v>
       </c>
       <c r="Q54" t="s">
-        <v>528</v>
+        <v>831</v>
       </c>
       <c r="R54" t="s">
-        <v>819</v>
+        <v>528</v>
       </c>
       <c r="S54" t="s">
         <v>72</v>
@@ -10399,7 +10405,7 @@
         <v>33</v>
       </c>
       <c r="V54" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="W54" t="s">
         <v>74</v>
@@ -10431,34 +10437,34 @@
         <v>827</v>
       </c>
       <c r="B55">
-        <v>115282</v>
+        <v>102870</v>
       </c>
       <c r="C55" t="s">
         <v>816</v>
       </c>
       <c r="D55" t="s">
-        <v>839</v>
+        <v>862</v>
       </c>
       <c r="E55" t="s">
-        <v>840</v>
+        <v>875</v>
       </c>
       <c r="F55" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="G55" t="s">
-        <v>852</v>
+        <v>876</v>
       </c>
       <c r="H55" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I55" t="s">
         <v>52</v>
       </c>
       <c r="J55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L55">
         <v>2</v>
@@ -10523,40 +10529,40 @@
         <v>827</v>
       </c>
       <c r="B56">
-        <v>93783</v>
+        <v>103173</v>
       </c>
       <c r="C56" t="s">
         <v>816</v>
       </c>
       <c r="D56" t="s">
-        <v>853</v>
+        <v>889</v>
       </c>
       <c r="E56" t="s">
-        <v>911</v>
+        <v>890</v>
       </c>
       <c r="F56" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
       <c r="G56" t="s">
-        <v>1117</v>
+        <v>921</v>
       </c>
       <c r="H56" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="I56" t="s">
         <v>52</v>
       </c>
       <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="K56">
         <v>3</v>
       </c>
-      <c r="K56">
-        <v>1</v>
-      </c>
       <c r="L56">
         <v>2</v>
       </c>
       <c r="M56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N56" t="s">
         <v>528</v>
@@ -10565,7 +10571,7 @@
         <v>528</v>
       </c>
       <c r="P56" t="s">
-        <v>528</v>
+        <v>838</v>
       </c>
       <c r="Q56" t="s">
         <v>528</v>
@@ -10574,13 +10580,13 @@
         <v>528</v>
       </c>
       <c r="S56" t="s">
-        <v>528</v>
+        <v>72</v>
       </c>
       <c r="T56" t="s">
-        <v>528</v>
+        <v>48</v>
       </c>
       <c r="U56" t="s">
-        <v>528</v>
+        <v>33</v>
       </c>
       <c r="V56" t="s">
         <v>1118</v>
@@ -10615,34 +10621,34 @@
         <v>827</v>
       </c>
       <c r="B57">
-        <v>102870</v>
+        <v>90222</v>
       </c>
       <c r="C57" t="s">
         <v>816</v>
       </c>
       <c r="D57" t="s">
-        <v>862</v>
+        <v>1051</v>
       </c>
       <c r="E57" t="s">
-        <v>875</v>
+        <v>1052</v>
       </c>
       <c r="F57" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="G57" t="s">
-        <v>876</v>
+        <v>1053</v>
       </c>
       <c r="H57" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I57" t="s">
         <v>52</v>
       </c>
       <c r="J57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L57">
         <v>2</v>
@@ -10663,7 +10669,7 @@
         <v>831</v>
       </c>
       <c r="R57" t="s">
-        <v>528</v>
+        <v>819</v>
       </c>
       <c r="S57" t="s">
         <v>72</v>
@@ -10675,7 +10681,7 @@
         <v>33</v>
       </c>
       <c r="V57" t="s">
-        <v>1664</v>
+        <v>1118</v>
       </c>
       <c r="W57" t="s">
         <v>74</v>
@@ -10707,22 +10713,22 @@
         <v>827</v>
       </c>
       <c r="B58">
-        <v>103173</v>
+        <v>121556</v>
       </c>
       <c r="C58" t="s">
         <v>816</v>
       </c>
       <c r="D58" t="s">
-        <v>889</v>
+        <v>828</v>
       </c>
       <c r="E58" t="s">
-        <v>890</v>
+        <v>829</v>
       </c>
       <c r="F58" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="G58" t="s">
-        <v>921</v>
+        <v>1110</v>
       </c>
       <c r="H58" t="s">
         <v>49</v>
@@ -10749,13 +10755,13 @@
         <v>528</v>
       </c>
       <c r="P58" t="s">
-        <v>838</v>
+        <v>528</v>
       </c>
       <c r="Q58" t="s">
         <v>528</v>
       </c>
       <c r="R58" t="s">
-        <v>528</v>
+        <v>819</v>
       </c>
       <c r="S58" t="s">
         <v>72</v>
@@ -10767,7 +10773,7 @@
         <v>33</v>
       </c>
       <c r="V58" t="s">
-        <v>1118</v>
+        <v>1663</v>
       </c>
       <c r="W58" t="s">
         <v>74</v>
@@ -10799,22 +10805,22 @@
         <v>827</v>
       </c>
       <c r="B59">
-        <v>90222</v>
+        <v>718238</v>
       </c>
       <c r="C59" t="s">
         <v>816</v>
       </c>
       <c r="D59" t="s">
-        <v>1051</v>
+        <v>853</v>
       </c>
       <c r="E59" t="s">
-        <v>1052</v>
+        <v>911</v>
       </c>
       <c r="F59" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="G59" t="s">
-        <v>1053</v>
+        <v>1113</v>
       </c>
       <c r="H59" t="s">
         <v>49</v>
@@ -10844,7 +10850,7 @@
         <v>528</v>
       </c>
       <c r="Q59" t="s">
-        <v>831</v>
+        <v>528</v>
       </c>
       <c r="R59" t="s">
         <v>819</v>
@@ -10859,7 +10865,7 @@
         <v>33</v>
       </c>
       <c r="V59" t="s">
-        <v>1118</v>
+        <v>1663</v>
       </c>
       <c r="W59" t="s">
         <v>74</v>
@@ -10891,22 +10897,22 @@
         <v>827</v>
       </c>
       <c r="B60">
-        <v>121556</v>
+        <v>80037</v>
       </c>
       <c r="C60" t="s">
         <v>816</v>
       </c>
       <c r="D60" t="s">
-        <v>828</v>
+        <v>845</v>
       </c>
       <c r="E60" t="s">
-        <v>829</v>
+        <v>846</v>
       </c>
       <c r="F60" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="G60" t="s">
-        <v>1110</v>
+        <v>1121</v>
       </c>
       <c r="H60" t="s">
         <v>49</v>
@@ -10983,7 +10989,7 @@
         <v>827</v>
       </c>
       <c r="B61">
-        <v>718238</v>
+        <v>138765</v>
       </c>
       <c r="C61" t="s">
         <v>816</v>
@@ -10992,13 +10998,13 @@
         <v>853</v>
       </c>
       <c r="E61" t="s">
-        <v>911</v>
+        <v>895</v>
       </c>
       <c r="F61" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="G61" t="s">
-        <v>1113</v>
+        <v>1122</v>
       </c>
       <c r="H61" t="s">
         <v>49</v>
@@ -11028,10 +11034,10 @@
         <v>528</v>
       </c>
       <c r="Q61" t="s">
-        <v>528</v>
+        <v>831</v>
       </c>
       <c r="R61" t="s">
-        <v>819</v>
+        <v>528</v>
       </c>
       <c r="S61" t="s">
         <v>72</v>
@@ -11043,7 +11049,7 @@
         <v>33</v>
       </c>
       <c r="V61" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="W61" t="s">
         <v>74</v>
@@ -11075,22 +11081,22 @@
         <v>827</v>
       </c>
       <c r="B62">
-        <v>80037</v>
+        <v>975602</v>
       </c>
       <c r="C62" t="s">
         <v>816</v>
       </c>
       <c r="D62" t="s">
-        <v>845</v>
+        <v>897</v>
       </c>
       <c r="E62" t="s">
-        <v>846</v>
+        <v>898</v>
       </c>
       <c r="F62" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="G62" t="s">
-        <v>1121</v>
+        <v>899</v>
       </c>
       <c r="H62" t="s">
         <v>49</v>
@@ -11117,13 +11123,13 @@
         <v>528</v>
       </c>
       <c r="P62" t="s">
-        <v>528</v>
+        <v>838</v>
       </c>
       <c r="Q62" t="s">
         <v>528</v>
       </c>
       <c r="R62" t="s">
-        <v>819</v>
+        <v>528</v>
       </c>
       <c r="S62" t="s">
         <v>72</v>
@@ -11135,7 +11141,7 @@
         <v>33</v>
       </c>
       <c r="V62" t="s">
-        <v>1663</v>
+        <v>1118</v>
       </c>
       <c r="W62" t="s">
         <v>74</v>
@@ -11167,40 +11173,40 @@
         <v>827</v>
       </c>
       <c r="B63">
-        <v>138765</v>
+        <v>94567</v>
       </c>
       <c r="C63" t="s">
         <v>816</v>
       </c>
       <c r="D63" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="E63" t="s">
-        <v>895</v>
+        <v>846</v>
       </c>
       <c r="F63" t="s">
-        <v>1237</v>
+        <v>1224</v>
       </c>
       <c r="G63" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="H63" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I63" t="s">
         <v>52</v>
       </c>
       <c r="J63">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L63">
         <v>2</v>
       </c>
       <c r="M63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N63" t="s">
         <v>528</v>
@@ -11212,22 +11218,22 @@
         <v>528</v>
       </c>
       <c r="Q63" t="s">
-        <v>831</v>
+        <v>528</v>
       </c>
       <c r="R63" t="s">
         <v>528</v>
       </c>
       <c r="S63" t="s">
-        <v>72</v>
+        <v>528</v>
       </c>
       <c r="T63" t="s">
-        <v>48</v>
+        <v>528</v>
       </c>
       <c r="U63" t="s">
-        <v>33</v>
+        <v>528</v>
       </c>
       <c r="V63" t="s">
-        <v>1664</v>
+        <v>1118</v>
       </c>
       <c r="W63" t="s">
         <v>74</v>
@@ -11259,40 +11265,40 @@
         <v>827</v>
       </c>
       <c r="B64">
-        <v>975602</v>
+        <v>92254</v>
       </c>
       <c r="C64" t="s">
         <v>816</v>
       </c>
       <c r="D64" t="s">
-        <v>897</v>
+        <v>868</v>
       </c>
       <c r="E64" t="s">
-        <v>898</v>
+        <v>869</v>
       </c>
       <c r="F64" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="G64" t="s">
-        <v>899</v>
+        <v>873</v>
       </c>
       <c r="H64" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I64" t="s">
         <v>52</v>
       </c>
       <c r="J64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K64">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L64">
         <v>2</v>
       </c>
       <c r="M64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N64" t="s">
         <v>528</v>
@@ -11301,7 +11307,7 @@
         <v>528</v>
       </c>
       <c r="P64" t="s">
-        <v>838</v>
+        <v>528</v>
       </c>
       <c r="Q64" t="s">
         <v>528</v>
@@ -11310,13 +11316,13 @@
         <v>528</v>
       </c>
       <c r="S64" t="s">
-        <v>72</v>
+        <v>528</v>
       </c>
       <c r="T64" t="s">
-        <v>48</v>
+        <v>528</v>
       </c>
       <c r="U64" t="s">
-        <v>33</v>
+        <v>528</v>
       </c>
       <c r="V64" t="s">
         <v>1118</v>
@@ -11343,7 +11349,7 @@
         <v>531</v>
       </c>
       <c r="AD64" t="s">
-        <v>528</v>
+        <v>820</v>
       </c>
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.25">
@@ -11351,31 +11357,31 @@
         <v>827</v>
       </c>
       <c r="B65">
-        <v>92254</v>
+        <v>93783</v>
       </c>
       <c r="C65" t="s">
         <v>816</v>
       </c>
       <c r="D65" t="s">
-        <v>868</v>
+        <v>853</v>
       </c>
       <c r="E65" t="s">
-        <v>869</v>
+        <v>911</v>
       </c>
       <c r="F65" t="s">
-        <v>1239</v>
+        <v>1230</v>
       </c>
       <c r="G65" t="s">
-        <v>873</v>
+        <v>1117</v>
       </c>
       <c r="H65" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="I65" t="s">
         <v>52</v>
       </c>
       <c r="J65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -11435,7 +11441,7 @@
         <v>531</v>
       </c>
       <c r="AD65" t="s">
-        <v>820</v>
+        <v>528</v>
       </c>
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.25">
@@ -42171,25 +42177,25 @@
         <v>238</v>
       </c>
       <c r="B400">
-        <v>4308</v>
+        <v>3603</v>
       </c>
       <c r="C400" t="s">
         <v>239</v>
       </c>
       <c r="D400" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E400" t="s">
-        <v>728</v>
+        <v>704</v>
       </c>
       <c r="F400" t="s">
-        <v>1569</v>
+        <v>1586</v>
       </c>
       <c r="G400" t="s">
-        <v>369</v>
+        <v>750</v>
       </c>
       <c r="H400" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I400" t="s">
         <v>49</v>
@@ -42204,7 +42210,7 @@
         <v>1</v>
       </c>
       <c r="M400">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N400" t="s">
         <v>528</v>
@@ -42228,7 +42234,7 @@
         <v>525</v>
       </c>
       <c r="U400" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="V400" t="s">
         <v>528</v>
@@ -42249,7 +42255,7 @@
         <v>528</v>
       </c>
       <c r="AB400" t="s">
-        <v>537</v>
+        <v>1674</v>
       </c>
       <c r="AC400" t="s">
         <v>528</v>
@@ -42263,25 +42269,25 @@
         <v>238</v>
       </c>
       <c r="B401">
-        <v>4319</v>
+        <v>3611</v>
       </c>
       <c r="C401" t="s">
         <v>239</v>
       </c>
       <c r="D401" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E401" t="s">
-        <v>721</v>
+        <v>704</v>
       </c>
       <c r="F401" t="s">
-        <v>1570</v>
+        <v>1587</v>
       </c>
       <c r="G401" t="s">
-        <v>370</v>
+        <v>409</v>
       </c>
       <c r="H401" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I401" t="s">
         <v>49</v>
@@ -42296,7 +42302,7 @@
         <v>1</v>
       </c>
       <c r="M401">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N401" t="s">
         <v>528</v>
@@ -42320,7 +42326,7 @@
         <v>525</v>
       </c>
       <c r="U401" t="s">
-        <v>133</v>
+        <v>33</v>
       </c>
       <c r="V401" t="s">
         <v>528</v>
@@ -42341,7 +42347,7 @@
         <v>528</v>
       </c>
       <c r="AB401" t="s">
-        <v>537</v>
+        <v>1675</v>
       </c>
       <c r="AC401" t="s">
         <v>528</v>
@@ -42355,7 +42361,7 @@
         <v>238</v>
       </c>
       <c r="B402">
-        <v>199425</v>
+        <v>4308</v>
       </c>
       <c r="C402" t="s">
         <v>239</v>
@@ -42364,13 +42370,13 @@
         <v>257</v>
       </c>
       <c r="E402" t="s">
-        <v>721</v>
+        <v>728</v>
       </c>
       <c r="F402" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="G402" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H402" t="s">
         <v>40</v>
@@ -42447,7 +42453,7 @@
         <v>238</v>
       </c>
       <c r="B403">
-        <v>4167</v>
+        <v>4319</v>
       </c>
       <c r="C403" t="s">
         <v>239</v>
@@ -42456,13 +42462,13 @@
         <v>257</v>
       </c>
       <c r="E403" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="F403" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="G403" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="H403" t="s">
         <v>40</v>
@@ -42531,7 +42537,7 @@
         <v>528</v>
       </c>
       <c r="AD403" t="s">
-        <v>284</v>
+        <v>528</v>
       </c>
     </row>
     <row r="404" spans="1:30" x14ac:dyDescent="0.25">
@@ -42539,7 +42545,7 @@
         <v>238</v>
       </c>
       <c r="B404">
-        <v>4254</v>
+        <v>199425</v>
       </c>
       <c r="C404" t="s">
         <v>239</v>
@@ -42548,13 +42554,13 @@
         <v>257</v>
       </c>
       <c r="E404" t="s">
-        <v>705</v>
+        <v>721</v>
       </c>
       <c r="F404" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="G404" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H404" t="s">
         <v>40</v>
@@ -42631,28 +42637,28 @@
         <v>238</v>
       </c>
       <c r="B405">
-        <v>3465</v>
+        <v>4167</v>
       </c>
       <c r="C405" t="s">
         <v>239</v>
       </c>
       <c r="D405" t="s">
-        <v>382</v>
+        <v>257</v>
       </c>
       <c r="E405" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="F405" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="G405" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="H405" t="s">
+        <v>40</v>
+      </c>
+      <c r="I405" t="s">
         <v>49</v>
-      </c>
-      <c r="I405" t="s">
-        <v>40</v>
       </c>
       <c r="J405">
         <v>1</v>
@@ -42715,7 +42721,7 @@
         <v>528</v>
       </c>
       <c r="AD405" t="s">
-        <v>528</v>
+        <v>284</v>
       </c>
     </row>
     <row r="406" spans="1:30" x14ac:dyDescent="0.25">
@@ -42723,7 +42729,7 @@
         <v>238</v>
       </c>
       <c r="B406">
-        <v>3784</v>
+        <v>4254</v>
       </c>
       <c r="C406" t="s">
         <v>239</v>
@@ -42732,25 +42738,25 @@
         <v>257</v>
       </c>
       <c r="E406" t="s">
-        <v>746</v>
+        <v>705</v>
       </c>
       <c r="F406" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="G406" t="s">
-        <v>400</v>
+        <v>374</v>
       </c>
       <c r="H406" t="s">
+        <v>40</v>
+      </c>
+      <c r="I406" t="s">
         <v>49</v>
       </c>
-      <c r="I406" t="s">
-        <v>40</v>
-      </c>
       <c r="J406">
         <v>1</v>
       </c>
       <c r="K406">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L406">
         <v>1</v>
@@ -42815,22 +42821,22 @@
         <v>238</v>
       </c>
       <c r="B407">
-        <v>534751</v>
+        <v>3465</v>
       </c>
       <c r="C407" t="s">
         <v>239</v>
       </c>
       <c r="D407" t="s">
-        <v>257</v>
+        <v>382</v>
       </c>
       <c r="E407" t="s">
-        <v>712</v>
+        <v>732</v>
       </c>
       <c r="F407" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="G407" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="H407" t="s">
         <v>49</v>
@@ -42907,7 +42913,7 @@
         <v>238</v>
       </c>
       <c r="B408">
-        <v>3774</v>
+        <v>3784</v>
       </c>
       <c r="C408" t="s">
         <v>239</v>
@@ -42916,13 +42922,13 @@
         <v>257</v>
       </c>
       <c r="E408" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F408" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="G408" t="s">
-        <v>748</v>
+        <v>400</v>
       </c>
       <c r="H408" t="s">
         <v>49</v>
@@ -42934,7 +42940,7 @@
         <v>1</v>
       </c>
       <c r="K408">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L408">
         <v>1</v>
@@ -42999,7 +43005,7 @@
         <v>238</v>
       </c>
       <c r="B409">
-        <v>4040</v>
+        <v>534751</v>
       </c>
       <c r="C409" t="s">
         <v>239</v>
@@ -43008,19 +43014,19 @@
         <v>257</v>
       </c>
       <c r="E409" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="F409" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="G409" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H409" t="s">
         <v>49</v>
       </c>
       <c r="I409" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J409">
         <v>1</v>
@@ -43091,7 +43097,7 @@
         <v>238</v>
       </c>
       <c r="B410">
-        <v>4625</v>
+        <v>3774</v>
       </c>
       <c r="C410" t="s">
         <v>239</v>
@@ -43100,19 +43106,19 @@
         <v>257</v>
       </c>
       <c r="E410" t="s">
-        <v>715</v>
+        <v>747</v>
       </c>
       <c r="F410" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="G410" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="H410" t="s">
         <v>49</v>
       </c>
       <c r="I410" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J410">
         <v>1</v>
@@ -43183,7 +43189,7 @@
         <v>238</v>
       </c>
       <c r="B411">
-        <v>1027359</v>
+        <v>4040</v>
       </c>
       <c r="C411" t="s">
         <v>239</v>
@@ -43192,13 +43198,13 @@
         <v>257</v>
       </c>
       <c r="E411" t="s">
-        <v>705</v>
+        <v>721</v>
       </c>
       <c r="F411" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="G411" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H411" t="s">
         <v>49</v>
@@ -43275,7 +43281,7 @@
         <v>238</v>
       </c>
       <c r="B412">
-        <v>4252</v>
+        <v>4625</v>
       </c>
       <c r="C412" t="s">
         <v>239</v>
@@ -43284,13 +43290,13 @@
         <v>257</v>
       </c>
       <c r="E412" t="s">
-        <v>705</v>
+        <v>715</v>
       </c>
       <c r="F412" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="G412" t="s">
-        <v>404</v>
+        <v>749</v>
       </c>
       <c r="H412" t="s">
         <v>49</v>
@@ -43367,7 +43373,7 @@
         <v>238</v>
       </c>
       <c r="B413">
-        <v>4659</v>
+        <v>1027359</v>
       </c>
       <c r="C413" t="s">
         <v>239</v>
@@ -43376,13 +43382,13 @@
         <v>257</v>
       </c>
       <c r="E413" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
       <c r="F413" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="G413" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H413" t="s">
         <v>49</v>
@@ -43459,7 +43465,7 @@
         <v>238</v>
       </c>
       <c r="B414">
-        <v>3941</v>
+        <v>4252</v>
       </c>
       <c r="C414" t="s">
         <v>239</v>
@@ -43468,13 +43474,13 @@
         <v>257</v>
       </c>
       <c r="E414" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="F414" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="G414" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H414" t="s">
         <v>49</v>
@@ -43551,7 +43557,7 @@
         <v>238</v>
       </c>
       <c r="B415">
-        <v>3755</v>
+        <v>4659</v>
       </c>
       <c r="C415" t="s">
         <v>239</v>
@@ -43560,13 +43566,13 @@
         <v>257</v>
       </c>
       <c r="E415" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="F415" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="G415" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H415" t="s">
         <v>49</v>
@@ -43643,7 +43649,7 @@
         <v>238</v>
       </c>
       <c r="B416">
-        <v>3741</v>
+        <v>3941</v>
       </c>
       <c r="C416" t="s">
         <v>239</v>
@@ -43655,10 +43661,10 @@
         <v>713</v>
       </c>
       <c r="F416" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="G416" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H416" t="s">
         <v>49</v>
@@ -43727,7 +43733,7 @@
         <v>528</v>
       </c>
       <c r="AD416" t="s">
-        <v>284</v>
+        <v>528</v>
       </c>
     </row>
     <row r="417" spans="1:30" x14ac:dyDescent="0.25">
@@ -43735,22 +43741,22 @@
         <v>238</v>
       </c>
       <c r="B417">
-        <v>3603</v>
+        <v>3755</v>
       </c>
       <c r="C417" t="s">
         <v>239</v>
       </c>
       <c r="D417" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E417" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F417" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="G417" t="s">
-        <v>750</v>
+        <v>407</v>
       </c>
       <c r="H417" t="s">
         <v>49</v>
@@ -43827,22 +43833,22 @@
         <v>238</v>
       </c>
       <c r="B418">
-        <v>3611</v>
+        <v>3741</v>
       </c>
       <c r="C418" t="s">
         <v>239</v>
       </c>
       <c r="D418" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E418" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="F418" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="G418" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H418" t="s">
         <v>49</v>
@@ -43911,7 +43917,7 @@
         <v>528</v>
       </c>
       <c r="AD418" t="s">
-        <v>528</v>
+        <v>284</v>
       </c>
     </row>
     <row r="419" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>